<commit_message>
#212 Update notebook 3
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
@@ -33,12 +33,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>market_cap</t>
-  </si>
-  <si>
-    <t>cash_equivalents</t>
-  </si>
-  <si>
     <t>Advanced Micro Devices, Inc</t>
   </si>
   <si>
@@ -580,13 +574,19 @@
   </si>
   <si>
     <t>base_year_ghg_s3</t>
+  </si>
+  <si>
+    <t>company_market_cap</t>
+  </si>
+  <si>
+    <t>company_cash_equivalents</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,6 +601,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
     </font>
   </fonts>
   <fills count="2">
@@ -623,9 +628,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -671,12 +679,12 @@
     <tableColumn id="18" name="ghg_s1s2"/>
     <tableColumn id="8" name="ghg_s3"/>
     <tableColumn id="9" name="company_revenue"/>
-    <tableColumn id="10" name="market_cap"/>
+    <tableColumn id="10" name="company_market_cap"/>
     <tableColumn id="11" name="company_enterprise_value"/>
     <tableColumn id="12" name="company_total_assets" dataDxfId="0">
-      <calculatedColumnFormula>Table1[[#This Row],[market_cap]]*Q2</calculatedColumnFormula>
+      <calculatedColumnFormula>Table1[[#This Row],[company_market_cap]]*Q2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" name="cash_equivalents"/>
+    <tableColumn id="13" name="company_cash_equivalents"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -972,11 +980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -989,74 +997,74 @@
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E1" t="s">
+        <v>166</v>
+      </c>
+      <c r="F1" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" t="s">
+        <v>169</v>
+      </c>
+      <c r="I1" t="s">
+        <v>170</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" t="s">
+        <v>172</v>
+      </c>
+      <c r="M1" t="s">
+        <v>173</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="O1" t="s">
         <v>162</v>
       </c>
-      <c r="C1" t="s">
-        <v>166</v>
-      </c>
-      <c r="D1" t="s">
-        <v>167</v>
-      </c>
-      <c r="E1" t="s">
-        <v>168</v>
-      </c>
-      <c r="F1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G1" t="s">
-        <v>170</v>
-      </c>
-      <c r="H1" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>173</v>
-      </c>
-      <c r="L1" t="s">
-        <v>174</v>
-      </c>
-      <c r="M1" t="s">
-        <v>175</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="P1" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="O1" t="s">
-        <v>164</v>
-      </c>
-      <c r="P1" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
-      </c>
-      <c r="E2" t="s">
-        <v>7</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
       </c>
       <c r="K2">
         <v>24965246.128183831</v>
@@ -1080,21 +1088,21 @@
         <v>4528467714.7267609</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" t="s">
         <v>9</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="J3" t="s">
-        <v>11</v>
       </c>
       <c r="K3">
         <v>1288468.9201645069</v>
@@ -1118,21 +1126,21 @@
         <v>69006940.998092517</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
+      <c r="J4" t="s">
         <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
       </c>
       <c r="K4">
         <v>230191.46897492089</v>
@@ -1156,21 +1164,21 @@
         <v>1163119848.4230556</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="J5" t="s">
         <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
       </c>
       <c r="K5">
         <v>178705.06184309252</v>
@@ -1194,21 +1202,21 @@
         <v>117630751.45422383</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" t="s">
         <v>19</v>
       </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K6">
         <v>97771.835813462851</v>
@@ -1232,21 +1240,21 @@
         <v>28933197273.168182</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
         <v>23</v>
-      </c>
-      <c r="D7" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>7</v>
-      </c>
-      <c r="J7" t="s">
-        <v>25</v>
       </c>
       <c r="K7">
         <v>466041.10015869705</v>
@@ -1270,21 +1278,21 @@
         <v>51876930016.314178</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K8">
         <v>128250.99022235045</v>
@@ -1308,21 +1316,21 @@
         <v>2214490.9702577037</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="J9" t="s">
         <v>28</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" t="s">
-        <v>7</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
       </c>
       <c r="K9">
         <v>1736.1153986195452</v>
@@ -1346,21 +1354,21 @@
         <v>203940251.11854151</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="J10" t="s">
         <v>33</v>
-      </c>
-      <c r="E10" t="s">
-        <v>34</v>
-      </c>
-      <c r="J10" t="s">
-        <v>35</v>
       </c>
       <c r="K10">
         <v>196777.12553570265</v>
@@ -1384,21 +1392,21 @@
         <v>42950453116.50563</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J11" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K11">
         <v>259165.86622702488</v>
@@ -1422,21 +1430,21 @@
         <v>5520000408.4878492</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J12" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K12">
         <v>81810.361536814045</v>
@@ -1460,21 +1468,21 @@
         <v>505519258.45795137</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="B13" t="s">
-        <v>41</v>
-      </c>
-      <c r="D13" t="s">
-        <v>42</v>
-      </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K13">
         <v>14847.919278129972</v>
@@ -1498,21 +1506,21 @@
         <v>462245314.11453331</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J14" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K14">
         <v>31895.87194649009</v>
@@ -1536,21 +1544,21 @@
         <v>1853875026.0311818</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K15">
         <v>42305.282163536431</v>
@@ -1574,21 +1582,21 @@
         <v>3272481697.8285317</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
         <v>47</v>
       </c>
-      <c r="B16" t="s">
-        <v>48</v>
-      </c>
-      <c r="D16" t="s">
-        <v>49</v>
-      </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J16" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K16">
         <v>118561.91297201814</v>
@@ -1612,21 +1620,21 @@
         <v>518880676.89759755</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J17" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K17">
         <v>45833216.792469583</v>
@@ -1650,21 +1658,21 @@
         <v>990719858.47337103</v>
       </c>
     </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K18">
         <v>9600.4773434214167</v>
@@ -1688,21 +1696,21 @@
         <v>470283632.88013947</v>
       </c>
     </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K19">
         <v>25428190.928034011</v>
@@ -1726,21 +1734,21 @@
         <v>963039844.50366735</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17">
       <c r="A20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" t="s">
         <v>56</v>
       </c>
-      <c r="B20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20" t="s">
-        <v>58</v>
-      </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J20" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K20">
         <v>85293.345618346313</v>
@@ -1764,21 +1772,21 @@
         <v>23467516.32994597</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17">
       <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21" t="s">
         <v>59</v>
       </c>
-      <c r="B21" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" t="s">
-        <v>61</v>
-      </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K21">
         <v>988.46631917228888</v>
@@ -1802,21 +1810,21 @@
         <v>457926390.7271148</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17">
       <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D22" t="s">
         <v>62</v>
       </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="D22" t="s">
-        <v>64</v>
-      </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J22" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K22">
         <v>20210717.506183945</v>
@@ -1840,21 +1848,21 @@
         <v>469617764.24836379</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B23" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D23" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J23" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K23">
         <v>2878524.2770361695</v>
@@ -1878,21 +1886,21 @@
         <v>209706066.63280141</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D24" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J24" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K24">
         <v>589526.73014329805</v>
@@ -1916,21 +1924,21 @@
         <v>80140338.552216381</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17">
       <c r="A25" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
         <v>69</v>
       </c>
-      <c r="B25" t="s">
-        <v>70</v>
-      </c>
-      <c r="D25" t="s">
-        <v>71</v>
-      </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J25" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K25">
         <v>7790.9166015573965</v>
@@ -1954,21 +1962,21 @@
         <v>1863069356.1369269</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E26" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K26">
         <v>2166428.3608621312</v>
@@ -1992,21 +2000,21 @@
         <v>802015633.4125073</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17">
       <c r="A27" t="s">
+        <v>72</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D27" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" t="s">
+        <v>32</v>
+      </c>
+      <c r="J27" t="s">
         <v>74</v>
-      </c>
-      <c r="B27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D27" t="s">
-        <v>71</v>
-      </c>
-      <c r="E27" t="s">
-        <v>34</v>
-      </c>
-      <c r="J27" t="s">
-        <v>76</v>
       </c>
       <c r="K27">
         <v>1374527.5713624337</v>
@@ -2030,21 +2038,21 @@
         <v>1090445581.1975896</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17">
       <c r="A28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B28" t="s">
+        <v>76</v>
+      </c>
+      <c r="D28" t="s">
         <v>77</v>
       </c>
-      <c r="B28" t="s">
+      <c r="E28" t="s">
         <v>78</v>
       </c>
-      <c r="D28" t="s">
-        <v>79</v>
-      </c>
-      <c r="E28" t="s">
-        <v>80</v>
-      </c>
       <c r="J28" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K28">
         <v>36340.85512554364</v>
@@ -2068,21 +2076,21 @@
         <v>408632883.32140654</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17">
       <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+      <c r="E29" t="s">
+        <v>78</v>
+      </c>
+      <c r="J29" t="s">
         <v>81</v>
-      </c>
-      <c r="B29" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>79</v>
-      </c>
-      <c r="E29" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" t="s">
-        <v>83</v>
       </c>
       <c r="K29">
         <v>68737.202118534289</v>
@@ -2106,21 +2114,21 @@
         <v>223357269.54921383</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17">
       <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" t="s">
+        <v>77</v>
+      </c>
+      <c r="E30" t="s">
+        <v>78</v>
+      </c>
+      <c r="J30" t="s">
         <v>84</v>
-      </c>
-      <c r="B30" t="s">
-        <v>85</v>
-      </c>
-      <c r="D30" t="s">
-        <v>79</v>
-      </c>
-      <c r="E30" t="s">
-        <v>80</v>
-      </c>
-      <c r="J30" t="s">
-        <v>86</v>
       </c>
       <c r="K30">
         <v>100484.3202610756</v>
@@ -2144,21 +2152,21 @@
         <v>1279584288.1275206</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17">
       <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="D31" t="s">
         <v>87</v>
       </c>
-      <c r="B31" t="s">
-        <v>88</v>
-      </c>
-      <c r="D31" t="s">
-        <v>89</v>
-      </c>
       <c r="E31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J31" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K31">
         <v>14088280.445939962</v>
@@ -2182,21 +2190,21 @@
         <v>259739897.26190066</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E32" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J32" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K32">
         <v>118941.23272573021</v>
@@ -2220,21 +2228,21 @@
         <v>2957267010.5849843</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B33" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J33" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K33">
         <v>21988.936351392673</v>
@@ -2258,21 +2266,21 @@
         <v>3249873922.9934068</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17">
       <c r="A34" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B34" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D34" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J34" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K34">
         <v>11935572.900812317</v>
@@ -2296,21 +2304,21 @@
         <v>1054147392.1400725</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17">
       <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="D35" t="s">
         <v>96</v>
       </c>
-      <c r="B35" t="s">
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" t="s">
         <v>97</v>
-      </c>
-      <c r="D35" t="s">
-        <v>98</v>
-      </c>
-      <c r="E35" t="s">
-        <v>7</v>
-      </c>
-      <c r="J35" t="s">
-        <v>99</v>
       </c>
       <c r="K35">
         <v>2107.7428559933919</v>
@@ -2334,21 +2342,21 @@
         <v>16164035.009301951</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17">
       <c r="A36" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J36" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K36">
         <v>314936.79875185777</v>
@@ -2372,21 +2380,21 @@
         <v>76375335.415532187</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B37" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J37" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K37">
         <v>91117.578012331389</v>
@@ -2410,21 +2418,21 @@
         <v>403556882.32980388</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17">
       <c r="A38" t="s">
+        <v>102</v>
+      </c>
+      <c r="B38" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E38" t="s">
+        <v>5</v>
+      </c>
+      <c r="J38" t="s">
         <v>104</v>
-      </c>
-      <c r="B38" t="s">
-        <v>105</v>
-      </c>
-      <c r="D38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E38" t="s">
-        <v>7</v>
-      </c>
-      <c r="J38" t="s">
-        <v>106</v>
       </c>
       <c r="K38">
         <v>26.865407941423623</v>
@@ -2448,21 +2456,21 @@
         <v>359922992.06079412</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:17">
       <c r="A39" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B39" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E39" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K39">
         <v>1988.9893256430512</v>
@@ -2486,21 +2494,21 @@
         <v>188775849.06628573</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:17">
       <c r="A40" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B40" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E40" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K40">
         <v>116613.16602106349</v>
@@ -2524,21 +2532,21 @@
         <v>3126017043.1166129</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:17">
       <c r="A41" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B41" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D41" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E41" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="J41" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K41">
         <v>2641303.9499925142</v>
@@ -2562,21 +2570,21 @@
         <v>25963862784.153816</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:17">
       <c r="A42" t="s">
+        <v>111</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" t="s">
         <v>113</v>
       </c>
-      <c r="B42" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" t="s">
-        <v>115</v>
-      </c>
       <c r="E42" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J42" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K42">
         <v>34886.045315286356</v>
@@ -2600,21 +2608,21 @@
         <v>216444951.50947747</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:17">
       <c r="A43" t="s">
+        <v>114</v>
+      </c>
+      <c r="B43" t="s">
+        <v>115</v>
+      </c>
+      <c r="D43" t="s">
         <v>116</v>
       </c>
-      <c r="B43" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" t="s">
-        <v>118</v>
-      </c>
       <c r="E43" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J43" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K43">
         <v>13266889.881567331</v>
@@ -2638,21 +2646,21 @@
         <v>463981837.16979945</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:17">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E44" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J44" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K44">
         <v>1436916.8962362793</v>
@@ -2676,21 +2684,21 @@
         <v>630827983.47226107</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17">
       <c r="A45" t="s">
+        <v>119</v>
+      </c>
+      <c r="B45" t="s">
+        <v>120</v>
+      </c>
+      <c r="D45" t="s">
         <v>121</v>
       </c>
-      <c r="B45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" t="s">
-        <v>123</v>
-      </c>
       <c r="E45" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J45" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K45">
         <v>6611043.5529440343</v>
@@ -2714,21 +2722,21 @@
         <v>1089931685.5934117</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:17">
       <c r="A46" t="s">
+        <v>122</v>
+      </c>
+      <c r="B46" t="s">
+        <v>123</v>
+      </c>
+      <c r="D46" t="s">
         <v>124</v>
       </c>
-      <c r="B46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D46" t="s">
-        <v>126</v>
-      </c>
       <c r="E46" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="J46" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="K46">
         <v>8307064.9522866216</v>
@@ -2752,21 +2760,21 @@
         <v>1580248549.8247914</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:17">
       <c r="A47" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D47" t="s">
         <v>127</v>
       </c>
-      <c r="B47" t="s">
+      <c r="E47" t="s">
         <v>128</v>
       </c>
-      <c r="D47" t="s">
-        <v>129</v>
-      </c>
-      <c r="E47" t="s">
-        <v>130</v>
-      </c>
       <c r="J47" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K47">
         <v>6086.1963717252083</v>
@@ -2790,21 +2798,21 @@
         <v>360167278.93933254</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:17">
       <c r="A48" t="s">
+        <v>129</v>
+      </c>
+      <c r="B48" t="s">
+        <v>130</v>
+      </c>
+      <c r="D48" t="s">
         <v>131</v>
       </c>
-      <c r="B48" t="s">
-        <v>132</v>
-      </c>
-      <c r="D48" t="s">
-        <v>133</v>
-      </c>
       <c r="E48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="J48" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="K48">
         <v>121886.58843968091</v>
@@ -2828,21 +2836,21 @@
         <v>23659060554.326973</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="A49" t="s">
+        <v>132</v>
+      </c>
+      <c r="B49" t="s">
+        <v>133</v>
+      </c>
+      <c r="D49" t="s">
         <v>134</v>
       </c>
-      <c r="B49" t="s">
-        <v>135</v>
-      </c>
-      <c r="D49" t="s">
-        <v>136</v>
-      </c>
       <c r="E49" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J49" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K49">
         <v>3073484.0384656894</v>
@@ -2866,21 +2874,21 @@
         <v>94976895574.746582</v>
       </c>
     </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:17">
       <c r="A50" t="s">
+        <v>135</v>
+      </c>
+      <c r="B50" t="s">
+        <v>136</v>
+      </c>
+      <c r="D50" t="s">
         <v>137</v>
       </c>
-      <c r="B50" t="s">
-        <v>138</v>
-      </c>
-      <c r="D50" t="s">
-        <v>139</v>
-      </c>
       <c r="E50" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="J50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="K50">
         <v>244176.80273373649</v>
@@ -2904,21 +2912,21 @@
         <v>408452279.29417968</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" t="s">
+        <v>138</v>
+      </c>
+      <c r="B51" t="s">
+        <v>139</v>
+      </c>
+      <c r="D51" t="s">
         <v>140</v>
       </c>
-      <c r="B51" t="s">
+      <c r="E51" t="s">
         <v>141</v>
       </c>
-      <c r="D51" t="s">
-        <v>142</v>
-      </c>
-      <c r="E51" t="s">
-        <v>143</v>
-      </c>
       <c r="J51" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="K51">
         <v>240504.60431777878</v>
@@ -2955,11 +2963,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2973,68 +2981,68 @@
     <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" t="s">
         <v>176</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>177</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>178</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>179</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M1" t="s">
         <v>180</v>
       </c>
-      <c r="H1" t="s">
+      <c r="N1" t="s">
         <v>181</v>
       </c>
-      <c r="I1" t="s">
-        <v>144</v>
-      </c>
-      <c r="J1" t="s">
-        <v>145</v>
-      </c>
-      <c r="K1" t="s">
+      <c r="O1" t="s">
+        <v>182</v>
+      </c>
+      <c r="P1" t="s">
         <v>146</v>
       </c>
-      <c r="L1" t="s">
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>147</v>
       </c>
-      <c r="M1" t="s">
-        <v>182</v>
-      </c>
-      <c r="N1" t="s">
-        <v>183</v>
-      </c>
-      <c r="O1" t="s">
-        <v>184</v>
-      </c>
-      <c r="P1" t="s">
+      <c r="E2" t="s">
         <v>148</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>149</v>
-      </c>
-      <c r="E2" t="s">
-        <v>150</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3064,21 +3072,21 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3109,21 +3117,21 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H4">
         <v>0.6</v>
@@ -3150,21 +3158,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D5" t="s">
+        <v>154</v>
+      </c>
+      <c r="E5" t="s">
         <v>151</v>
-      </c>
-      <c r="D5" t="s">
-        <v>156</v>
-      </c>
-      <c r="E5" t="s">
-        <v>153</v>
       </c>
       <c r="F5">
         <v>0.95</v>
@@ -3197,21 +3205,21 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D6" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" t="s">
         <v>151</v>
-      </c>
-      <c r="D6" t="s">
-        <v>156</v>
-      </c>
-      <c r="E6" t="s">
-        <v>153</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3244,21 +3252,21 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3288,18 +3296,18 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H8">
         <v>0.8</v>
@@ -3326,21 +3334,21 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3370,21 +3378,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3414,21 +3422,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D11" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3458,18 +3466,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3499,18 +3507,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -3540,18 +3548,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -3581,18 +3589,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3622,18 +3630,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17">
       <c r="A16" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E16" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3663,18 +3671,18 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16">
       <c r="A17" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E17" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3704,18 +3712,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E18" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H18">
         <v>0.12</v>
@@ -3742,18 +3750,18 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E19" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H19">
         <v>0.3</v>
@@ -3780,18 +3788,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16">
       <c r="A20" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E20" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H20">
         <v>0.4</v>
@@ -3818,18 +3826,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E21" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H21">
         <v>0.5</v>
@@ -3856,18 +3864,18 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16">
       <c r="A22" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B22" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H22">
         <v>0.6</v>
@@ -3894,18 +3902,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E23" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H23">
         <v>0.8</v>
@@ -3932,21 +3940,21 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B24" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H24">
         <v>0.7</v>
@@ -3973,18 +3981,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16">
       <c r="A25" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C25" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E25" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -4014,18 +4022,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16">
       <c r="A26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E26" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4055,21 +4063,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16">
       <c r="A27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D27" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E27" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F27">
         <v>0.95</v>
@@ -4099,21 +4107,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16">
       <c r="A28" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B28" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H28">
         <v>0.8</v>
@@ -4134,21 +4142,21 @@
         <v>0.49600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16">
       <c r="A29" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C29" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H29">
         <v>0.9</v>
@@ -4175,18 +4183,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16">
       <c r="A30" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B30" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C30" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F30">
         <v>0.99</v>
@@ -4216,21 +4224,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16">
       <c r="A31" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C31" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D31" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H31">
         <v>0.81</v>
@@ -4257,18 +4265,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C32" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E32" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F32">
         <v>0.85</v>
@@ -4298,18 +4306,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B33" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E33" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -4336,21 +4344,21 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D34" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E34" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -4377,18 +4385,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16">
       <c r="A35" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C35" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -4412,18 +4420,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E36" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4453,21 +4461,21 @@
         <v>6.1699999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16">
       <c r="A37" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C37" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D37" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H37">
         <v>0.159</v>
@@ -4494,21 +4502,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16">
       <c r="A38" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B38" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H38">
         <v>0.75</v>
@@ -4535,18 +4543,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16">
       <c r="A39" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B39" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E39" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -4573,21 +4581,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16">
       <c r="A40" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F40">
         <v>0.71</v>
@@ -4611,21 +4619,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16">
       <c r="A41" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B41" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C41" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D41" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E41" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F41">
         <v>0.75</v>
@@ -4655,21 +4663,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C42" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E42" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -4699,18 +4707,18 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16">
       <c r="A43" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B43" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C43" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4740,18 +4748,18 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16">
       <c r="A44" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E44" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F44">
         <v>0.86</v>
@@ -4781,18 +4789,18 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E45" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F45">
         <v>0.86</v>
@@ -4822,21 +4830,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16">
       <c r="A46" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C46" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D46" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E46" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4866,21 +4874,21 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16">
       <c r="A47" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C47" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D47" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E47" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4910,18 +4918,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16">
       <c r="A48" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B48" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C48" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E48" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F48">
         <v>0.65</v>
@@ -4951,21 +4959,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16">
       <c r="A49" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B49" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E49" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F49">
         <v>0.65</v>
@@ -4995,21 +5003,21 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16">
       <c r="A50" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D50" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E50" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F50">
         <v>0.65</v>
@@ -5042,18 +5050,18 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16">
       <c r="A51" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B51" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C51" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E51" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -5083,21 +5091,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B52" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C52" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D52" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E52" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -5124,21 +5132,21 @@
         <v>0.32600000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16">
       <c r="A53" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B53" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C53" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E53" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -5168,18 +5176,18 @@
         <v>5.4000000000000006E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16">
       <c r="A54" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B54" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C54" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E54" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F54">
         <v>0.7</v>
@@ -5209,18 +5217,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16">
       <c r="A55" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B55" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C55" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E55" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -5250,18 +5258,18 @@
         <v>0.30809999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16">
       <c r="A56" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B56" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C56" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E56" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -5291,18 +5299,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C57" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E57" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F57">
         <v>0.97</v>
@@ -5332,18 +5340,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16">
       <c r="A58" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B58" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C58" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E58" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -5373,21 +5381,21 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16">
       <c r="A59" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D59" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E59" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -5417,21 +5425,21 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16">
       <c r="A60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B60" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C60" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D60" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E60" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F60">
         <v>0.75</v>
@@ -5461,21 +5469,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B61" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D61" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E61" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -5505,18 +5513,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16">
       <c r="A62" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B62" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C62" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E62" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5546,18 +5554,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16">
       <c r="A63" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B63" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C63" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E63" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5587,18 +5595,18 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16">
       <c r="A64" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B64" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E64" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F64">
         <v>0.95</v>
@@ -5628,21 +5636,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C65" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D65" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E65" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F65">
         <v>0.95</v>
@@ -5672,21 +5680,21 @@
         <v>0.47789999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16">
       <c r="A66" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C66" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D66" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E66" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F66">
         <v>0.93</v>
@@ -5716,18 +5724,18 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16">
       <c r="A67" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B67" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C67" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E67" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -5757,21 +5765,21 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16">
       <c r="A68" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B68" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C68" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D68" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E68" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -5801,18 +5809,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16">
       <c r="A69" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C69" t="s">
+        <v>155</v>
+      </c>
+      <c r="E69" t="s">
         <v>157</v>
-      </c>
-      <c r="E69" t="s">
-        <v>159</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -5839,18 +5847,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B70" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C70" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E70" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -5880,21 +5888,21 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16">
       <c r="A71" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B71" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C71" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D71" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E71" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -5924,21 +5932,21 @@
         <v>6.4100000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16">
       <c r="A72" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B72" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C72" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D72" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E72" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H72">
         <v>0.7</v>
@@ -5965,18 +5973,18 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16">
       <c r="A73" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B73" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C73" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E73" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -6006,21 +6014,21 @@
         <v>0.11220000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16">
       <c r="A74" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B74" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C74" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D74" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E74" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -6050,18 +6058,18 @@
         <v>0.22870000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16">
       <c r="A75" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C75" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E75" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -6091,21 +6099,21 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16">
       <c r="A76" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C76" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D76" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E76" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6135,21 +6143,21 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C77" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D77" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E77" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6179,21 +6187,21 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16">
       <c r="A78" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B78" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D78" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E78" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6223,18 +6231,18 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C79" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E79" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H79">
         <v>0.95</v>
@@ -6261,21 +6269,21 @@
         <v>0.84400000000000008</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16">
       <c r="A80" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B80" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C80" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D80" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E80" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -6308,21 +6316,21 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16">
       <c r="A81" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B81" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C81" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D81" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6352,21 +6360,21 @@
         <v>0.55670000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16">
       <c r="A82" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B82" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C82" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D82" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E82" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -6393,21 +6401,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16">
       <c r="A83" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B83" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C83" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D83" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E83" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H83">
         <v>0.6</v>
@@ -6434,21 +6442,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16">
       <c r="A84" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B84" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C84" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D84" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E84" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H84">
         <v>0.95</v>
@@ -6475,18 +6483,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16">
       <c r="A85" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B85" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C85" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E85" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -6516,18 +6524,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16">
       <c r="A86" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B86" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C86" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E86" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H86">
         <v>0.89270000000000005</v>
@@ -6554,21 +6562,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16">
       <c r="A87" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C87" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D87" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E87" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F87">
         <v>0.93100000000000005</v>
@@ -6598,18 +6606,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16">
       <c r="A88" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B88" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C88" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E88" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G88">
         <v>0.04</v>
@@ -6636,21 +6644,21 @@
         <v>0.36700000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16">
       <c r="A89" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B89" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C89" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D89" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E89" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G89">
         <v>0.7</v>
@@ -6677,18 +6685,18 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16">
       <c r="A90" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B90" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C90" t="s">
+        <v>155</v>
+      </c>
+      <c r="E90" t="s">
         <v>157</v>
-      </c>
-      <c r="E90" t="s">
-        <v>159</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -6715,18 +6723,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16">
       <c r="A91" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B91" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C91" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E91" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -6753,18 +6761,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16">
       <c r="A92" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B92" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C92" t="s">
+        <v>155</v>
+      </c>
+      <c r="E92" t="s">
         <v>157</v>
-      </c>
-      <c r="E92" t="s">
-        <v>159</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -6791,18 +6799,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16">
       <c r="A93" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B93" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C93" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E93" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -6829,18 +6837,18 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16">
       <c r="A94" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B94" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C94" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E94" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -6870,18 +6878,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16">
       <c r="A95" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C95" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E95" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -6911,21 +6919,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16">
       <c r="A96" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B96" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C96" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D96" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E96" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -6955,21 +6963,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16">
       <c r="A97" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B97" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C97" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D97" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E97" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -6999,18 +7007,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16">
       <c r="A98" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B98" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C98" t="s">
+        <v>155</v>
+      </c>
+      <c r="E98" t="s">
         <v>157</v>
-      </c>
-      <c r="E98" t="s">
-        <v>159</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7037,18 +7045,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16">
       <c r="A99" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B99" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C99" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E99" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -7075,21 +7083,21 @@
         <v>0.82000000000000006</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16">
       <c r="A100" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B100" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C100" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D100" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E100" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F100">
         <v>0.87</v>
@@ -7119,18 +7127,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16">
       <c r="A101" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B101" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C101" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E101" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -7157,18 +7165,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16">
       <c r="A102" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B102" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C102" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E102" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F102">
         <v>0.27</v>
@@ -7198,21 +7206,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16">
       <c r="A103" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B103" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C103" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D103" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E103" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -7242,21 +7250,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16">
       <c r="A104" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B104" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C104" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D104" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E104" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -7286,21 +7294,21 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16">
       <c r="A105" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B105" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C105" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D105" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E105" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H105">
         <v>0.44</v>
@@ -7327,21 +7335,21 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16">
       <c r="A106" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B106" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C106" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D106" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E106" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -7371,18 +7379,18 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16">
       <c r="A107" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B107" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C107" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E107" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F107">
         <v>0.94</v>
@@ -7412,18 +7420,18 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16">
       <c r="A108" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B108" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C108" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E108" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F108">
         <v>0.94</v>
@@ -7453,21 +7461,21 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16">
       <c r="A109" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B109" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C109" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D109" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E109" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F109">
         <v>0.94</v>
@@ -7497,21 +7505,21 @@
         <v>0.57020000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16">
       <c r="A110" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B110" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C110" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D110" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E110" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -7538,21 +7546,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16">
       <c r="A111" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B111" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C111" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D111" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E111" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F111">
         <v>0.99</v>
@@ -7579,18 +7587,18 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16">
       <c r="A112" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B112" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C112" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E112" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -7620,21 +7628,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16">
       <c r="A113" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B113" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C113" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D113" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E113" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -7661,18 +7669,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16">
       <c r="A114" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B114" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C114" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E114" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F114">
         <v>0.99</v>
@@ -7702,18 +7710,18 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16">
       <c r="A115" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B115" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C115" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E115" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -7743,18 +7751,18 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16">
       <c r="A116" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B116" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C116" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E116" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F116">
         <v>0.66839999999999999</v>
@@ -7784,21 +7792,21 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16">
       <c r="A117" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B117" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C117" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D117" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E117" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F117">
         <v>0.2024</v>
@@ -7828,21 +7836,21 @@
         <v>0.154</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16">
       <c r="A118" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B118" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C118" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D118" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E118" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F118">
         <v>0.66900000000000004</v>
@@ -7872,18 +7880,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16">
       <c r="A119" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B119" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C119" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E119" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -7913,21 +7921,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16">
       <c r="A120" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B120" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C120" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D120" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E120" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F120">
         <v>0.6</v>

</xml_diff>

<commit_message>
update analysis & anonymize data
</commit_message>
<xml_diff>
--- a/examples/data/data_provider_example.xlsx
+++ b/examples/data/data_provider_example.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JanThiemenP\development\SBTi\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\src\SBTi\examples\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="fundamental_data" sheetId="1" r:id="rId1"/>
     <sheet name="target_data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +33,6 @@
     <t>sector</t>
   </si>
   <si>
-    <t>Advanced Micro Devices, Inc</t>
-  </si>
-  <si>
     <t>US0079031078</t>
   </si>
   <si>
@@ -48,18 +45,12 @@
     <t>Industrials</t>
   </si>
   <si>
-    <t>Adobe Systems Inc.</t>
-  </si>
-  <si>
     <t>US00724F1012</t>
   </si>
   <si>
     <t>Utilities</t>
   </si>
   <si>
-    <t>Capgemini Group</t>
-  </si>
-  <si>
     <t>FR0000125338</t>
   </si>
   <si>
@@ -72,24 +63,15 @@
     <t>Consumer Discretionary</t>
   </si>
   <si>
-    <t>Cisco Systems, Inc.</t>
-  </si>
-  <si>
     <t>US17275R1023</t>
   </si>
   <si>
-    <t>Coca-Cola HBC AG</t>
-  </si>
-  <si>
     <t>CH0198251305</t>
   </si>
   <si>
     <t>Switzerland</t>
   </si>
   <si>
-    <t>CVS Health</t>
-  </si>
-  <si>
     <t>US1266501006</t>
   </si>
   <si>
@@ -99,24 +81,15 @@
     <t>Health Care</t>
   </si>
   <si>
-    <t>Danone</t>
-  </si>
-  <si>
     <t>FR0000120644</t>
   </si>
   <si>
-    <t>Dell Technologies</t>
-  </si>
-  <si>
     <t>US24703L1035</t>
   </si>
   <si>
     <t>Financials</t>
   </si>
   <si>
-    <t>Delta Electronics</t>
-  </si>
-  <si>
     <t>TW0002308004</t>
   </si>
   <si>
@@ -129,57 +102,33 @@
     <t>Information Technology</t>
   </si>
   <si>
-    <t>L'Oréal</t>
-  </si>
-  <si>
     <t>FR0000120321</t>
   </si>
   <si>
-    <t>Nestlé</t>
-  </si>
-  <si>
     <t>CH0038863350</t>
   </si>
   <si>
-    <t>Sony Corporation</t>
-  </si>
-  <si>
     <t>US8356993076</t>
   </si>
   <si>
     <t>Japan</t>
   </si>
   <si>
-    <t>SUMITOMO CHEMICAL Co., Ltd.</t>
-  </si>
-  <si>
     <t>JP3401400001</t>
   </si>
   <si>
-    <t>NIKE, Inc.</t>
-  </si>
-  <si>
     <t>US6541061031</t>
   </si>
   <si>
-    <t>Marks &amp; Spencer</t>
-  </si>
-  <si>
     <t>GB0031274896</t>
   </si>
   <si>
     <t>United Kingdom</t>
   </si>
   <si>
-    <t>NRG Energy Inc</t>
-  </si>
-  <si>
     <t>US6293775085</t>
   </si>
   <si>
-    <t>PepsiCo, Inc.</t>
-  </si>
-  <si>
     <t>US7134481081</t>
   </si>
   <si>
@@ -580,13 +529,64 @@
   </si>
   <si>
     <t>company_cash_equivalents</t>
+  </si>
+  <si>
+    <t>Company AH</t>
+  </si>
+  <si>
+    <t>Company AI</t>
+  </si>
+  <si>
+    <t>Company AJ</t>
+  </si>
+  <si>
+    <t>Company AK</t>
+  </si>
+  <si>
+    <t>Company AL</t>
+  </si>
+  <si>
+    <t>Company AM</t>
+  </si>
+  <si>
+    <t>Company AN</t>
+  </si>
+  <si>
+    <t>Company AO</t>
+  </si>
+  <si>
+    <t>Company AP</t>
+  </si>
+  <si>
+    <t>Company AQ</t>
+  </si>
+  <si>
+    <t>Company AR</t>
+  </si>
+  <si>
+    <t>Company AS</t>
+  </si>
+  <si>
+    <t>Company AT</t>
+  </si>
+  <si>
+    <t>Company AU</t>
+  </si>
+  <si>
+    <t>Company AV</t>
+  </si>
+  <si>
+    <t>Company AX</t>
+  </si>
+  <si>
+    <t>Company AW</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -980,11 +980,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
@@ -997,74 +997,74 @@
     <col min="17" max="17" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>160</v>
+        <v>143</v>
       </c>
       <c r="C1" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D1" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" t="s">
+        <v>151</v>
+      </c>
+      <c r="H1" t="s">
+        <v>152</v>
+      </c>
+      <c r="I1" t="s">
+        <v>153</v>
+      </c>
+      <c r="J1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" t="s">
+        <v>154</v>
+      </c>
+      <c r="L1" t="s">
+        <v>155</v>
+      </c>
+      <c r="M1" t="s">
+        <v>156</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="F1" t="s">
+      <c r="O1" t="s">
+        <v>145</v>
+      </c>
+      <c r="P1" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q1" t="s">
         <v>167</v>
       </c>
-      <c r="G1" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" t="s">
-        <v>169</v>
-      </c>
-      <c r="I1" t="s">
-        <v>170</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" t="s">
-        <v>171</v>
-      </c>
-      <c r="L1" t="s">
-        <v>172</v>
-      </c>
-      <c r="M1" t="s">
-        <v>173</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>183</v>
-      </c>
-      <c r="O1" t="s">
-        <v>162</v>
-      </c>
-      <c r="P1" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="s">
+      <c r="J2" t="s">
         <v>5</v>
-      </c>
-      <c r="J2" t="s">
-        <v>6</v>
       </c>
       <c r="K2">
         <v>24965246.128183831</v>
@@ -1088,21 +1088,21 @@
         <v>4528467714.7267609</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" t="s">
         <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" t="s">
-        <v>9</v>
       </c>
       <c r="K3">
         <v>1288468.9201645069</v>
@@ -1126,21 +1126,21 @@
         <v>69006940.998092517</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="J4" t="s">
         <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" t="s">
-        <v>14</v>
       </c>
       <c r="K4">
         <v>230191.46897492089</v>
@@ -1164,21 +1164,21 @@
         <v>1163119848.4230556</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" t="s">
+      <c r="J5" t="s">
         <v>5</v>
-      </c>
-      <c r="J5" t="s">
-        <v>6</v>
       </c>
       <c r="K5">
         <v>178705.06184309252</v>
@@ -1202,21 +1202,21 @@
         <v>117630751.45422383</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K6">
         <v>97771.835813462851</v>
@@ -1240,21 +1240,21 @@
         <v>28933197273.168182</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J7" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K7">
         <v>466041.10015869705</v>
@@ -1278,21 +1278,21 @@
         <v>51876930016.314178</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K8">
         <v>128250.99022235045</v>
@@ -1316,21 +1316,21 @@
         <v>2214490.9702577037</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>1736.1153986195452</v>
@@ -1354,21 +1354,21 @@
         <v>203940251.11854151</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J10" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K10">
         <v>196777.12553570265</v>
@@ -1392,21 +1392,21 @@
         <v>42950453116.50563</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J11" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K11">
         <v>259165.86622702488</v>
@@ -1430,21 +1430,21 @@
         <v>5520000408.4878492</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E12" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J12" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K12">
         <v>81810.361536814045</v>
@@ -1468,21 +1468,21 @@
         <v>505519258.45795137</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J13" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K13">
         <v>14847.919278129972</v>
@@ -1506,21 +1506,21 @@
         <v>462245314.11453331</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K14">
         <v>31895.87194649009</v>
@@ -1544,21 +1544,21 @@
         <v>1853875026.0311818</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J15" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K15">
         <v>42305.282163536431</v>
@@ -1582,21 +1582,21 @@
         <v>3272481697.8285317</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="E16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J16" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K16">
         <v>118561.91297201814</v>
@@ -1620,21 +1620,21 @@
         <v>518880676.89759755</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="D17" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K17">
         <v>45833216.792469583</v>
@@ -1658,21 +1658,21 @@
         <v>990719858.47337103</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D18" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J18" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K18">
         <v>9600.4773434214167</v>
@@ -1696,21 +1696,21 @@
         <v>470283632.88013947</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J19" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K19">
         <v>25428190.928034011</v>
@@ -1734,21 +1734,21 @@
         <v>963039844.50366735</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J20" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K20">
         <v>85293.345618346313</v>
@@ -1772,21 +1772,21 @@
         <v>23467516.32994597</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="E21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J21" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K21">
         <v>988.46631917228888</v>
@@ -1810,21 +1810,21 @@
         <v>457926390.7271148</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E22" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J22" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K22">
         <v>20210717.506183945</v>
@@ -1848,21 +1848,21 @@
         <v>469617764.24836379</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="B23" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D23" t="s">
-        <v>62</v>
+        <v>45</v>
       </c>
       <c r="E23" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J23" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K23">
         <v>2878524.2770361695</v>
@@ -1886,21 +1886,21 @@
         <v>209706066.63280141</v>
       </c>
     </row>
-    <row r="24" spans="1:17">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
       <c r="B24" t="s">
-        <v>66</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E24" t="s">
+        <v>4</v>
+      </c>
+      <c r="J24" t="s">
         <v>5</v>
-      </c>
-      <c r="J24" t="s">
-        <v>6</v>
       </c>
       <c r="K24">
         <v>589526.73014329805</v>
@@ -1924,21 +1924,21 @@
         <v>80140338.552216381</v>
       </c>
     </row>
-    <row r="25" spans="1:17">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J25" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K25">
         <v>7790.9166015573965</v>
@@ -1962,21 +1962,21 @@
         <v>1863069356.1369269</v>
       </c>
     </row>
-    <row r="26" spans="1:17">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B26" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J26" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="K26">
         <v>2166428.3608621312</v>
@@ -2000,21 +2000,21 @@
         <v>802015633.4125073</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J27" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K27">
         <v>1374527.5713624337</v>
@@ -2038,21 +2038,21 @@
         <v>1090445581.1975896</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="B28" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="D28" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E28" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="J28" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K28">
         <v>36340.85512554364</v>
@@ -2076,21 +2076,21 @@
         <v>408632883.32140654</v>
       </c>
     </row>
-    <row r="29" spans="1:17">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B29" t="s">
-        <v>80</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E29" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="J29" t="s">
-        <v>81</v>
+        <v>64</v>
       </c>
       <c r="K29">
         <v>68737.202118534289</v>
@@ -2114,21 +2114,21 @@
         <v>223357269.54921383</v>
       </c>
     </row>
-    <row r="30" spans="1:17">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E30" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="J30" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K30">
         <v>100484.3202610756</v>
@@ -2152,21 +2152,21 @@
         <v>1279584288.1275206</v>
       </c>
     </row>
-    <row r="31" spans="1:17">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>87</v>
+        <v>70</v>
       </c>
       <c r="E31" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="J31" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K31">
         <v>14088280.445939962</v>
@@ -2190,21 +2190,21 @@
         <v>259739897.26190066</v>
       </c>
     </row>
-    <row r="32" spans="1:17">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>88</v>
+        <v>71</v>
       </c>
       <c r="B32" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
       <c r="D32" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J32" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K32">
         <v>118941.23272573021</v>
@@ -2228,21 +2228,21 @@
         <v>2957267010.5849843</v>
       </c>
     </row>
-    <row r="33" spans="1:17">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="D33" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E33" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K33">
         <v>21988.936351392673</v>
@@ -2266,21 +2266,21 @@
         <v>3249873922.9934068</v>
       </c>
     </row>
-    <row r="34" spans="1:17">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>76</v>
       </c>
       <c r="D34" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E34" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J34" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K34">
         <v>11935572.900812317</v>
@@ -2304,21 +2304,21 @@
         <v>1054147392.1400725</v>
       </c>
     </row>
-    <row r="35" spans="1:17">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D35" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J35" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="K35">
         <v>2107.7428559933919</v>
@@ -2342,21 +2342,21 @@
         <v>16164035.009301951</v>
       </c>
     </row>
-    <row r="36" spans="1:17">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="D36" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J36" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="K36">
         <v>314936.79875185777</v>
@@ -2380,21 +2380,21 @@
         <v>76375335.415532187</v>
       </c>
     </row>
-    <row r="37" spans="1:17">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B37" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="D37" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E37" t="s">
+        <v>4</v>
+      </c>
+      <c r="J37" t="s">
         <v>5</v>
-      </c>
-      <c r="J37" t="s">
-        <v>6</v>
       </c>
       <c r="K37">
         <v>91117.578012331389</v>
@@ -2418,21 +2418,21 @@
         <v>403556882.32980388</v>
       </c>
     </row>
-    <row r="38" spans="1:17">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="D38" t="s">
-        <v>96</v>
+        <v>79</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J38" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="K38">
         <v>26.865407941423623</v>
@@ -2456,21 +2456,21 @@
         <v>359922992.06079412</v>
       </c>
     </row>
-    <row r="39" spans="1:17">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B39" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="D39" t="s">
+        <v>3</v>
+      </c>
+      <c r="E39" t="s">
         <v>4</v>
       </c>
-      <c r="E39" t="s">
-        <v>5</v>
-      </c>
       <c r="J39" t="s">
-        <v>104</v>
+        <v>87</v>
       </c>
       <c r="K39">
         <v>1988.9893256430512</v>
@@ -2494,21 +2494,21 @@
         <v>188775849.06628573</v>
       </c>
     </row>
-    <row r="40" spans="1:17">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="D40" t="s">
+        <v>3</v>
+      </c>
+      <c r="E40" t="s">
         <v>4</v>
       </c>
-      <c r="E40" t="s">
-        <v>5</v>
-      </c>
       <c r="J40" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K40">
         <v>116613.16602106349</v>
@@ -2532,21 +2532,21 @@
         <v>3126017043.1166129</v>
       </c>
     </row>
-    <row r="41" spans="1:17">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B41" t="s">
-        <v>110</v>
+        <v>93</v>
       </c>
       <c r="D41" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" t="s">
         <v>4</v>
       </c>
-      <c r="E41" t="s">
-        <v>5</v>
-      </c>
       <c r="J41" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K41">
         <v>2641303.9499925142</v>
@@ -2570,21 +2570,21 @@
         <v>25963862784.153816</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B42" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D42" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E42" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J42" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K42">
         <v>34886.045315286356</v>
@@ -2608,21 +2608,21 @@
         <v>216444951.50947747</v>
       </c>
     </row>
-    <row r="43" spans="1:17">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>114</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="E43" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J43" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K43">
         <v>13266889.881567331</v>
@@ -2646,21 +2646,21 @@
         <v>463981837.16979945</v>
       </c>
     </row>
-    <row r="44" spans="1:17">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="D44" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="E44" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J44" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K44">
         <v>1436916.8962362793</v>
@@ -2684,21 +2684,21 @@
         <v>630827983.47226107</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B45" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="D45" t="s">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="E45" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J45" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K45">
         <v>6611043.5529440343</v>
@@ -2722,21 +2722,21 @@
         <v>1089931685.5934117</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>122</v>
+        <v>105</v>
       </c>
       <c r="B46" t="s">
-        <v>123</v>
+        <v>106</v>
       </c>
       <c r="D46" t="s">
-        <v>124</v>
+        <v>107</v>
       </c>
       <c r="E46" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="J46" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="K46">
         <v>8307064.9522866216</v>
@@ -2760,21 +2760,21 @@
         <v>1580248549.8247914</v>
       </c>
     </row>
-    <row r="47" spans="1:17">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>108</v>
       </c>
       <c r="B47" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="J47" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="K47">
         <v>6086.1963717252083</v>
@@ -2798,21 +2798,21 @@
         <v>360167278.93933254</v>
       </c>
     </row>
-    <row r="48" spans="1:17">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>129</v>
+        <v>112</v>
       </c>
       <c r="B48" t="s">
-        <v>130</v>
+        <v>113</v>
       </c>
       <c r="D48" t="s">
-        <v>131</v>
+        <v>114</v>
       </c>
       <c r="E48" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="J48" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="K48">
         <v>121886.58843968091</v>
@@ -2836,21 +2836,21 @@
         <v>23659060554.326973</v>
       </c>
     </row>
-    <row r="49" spans="1:17">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>132</v>
+        <v>115</v>
       </c>
       <c r="B49" t="s">
-        <v>133</v>
+        <v>116</v>
       </c>
       <c r="D49" t="s">
-        <v>134</v>
+        <v>117</v>
       </c>
       <c r="E49" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J49" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K49">
         <v>3073484.0384656894</v>
@@ -2874,21 +2874,21 @@
         <v>94976895574.746582</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>135</v>
+        <v>118</v>
       </c>
       <c r="B50" t="s">
-        <v>136</v>
+        <v>119</v>
       </c>
       <c r="D50" t="s">
-        <v>137</v>
+        <v>120</v>
       </c>
       <c r="E50" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="J50" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="K50">
         <v>244176.80273373649</v>
@@ -2912,21 +2912,21 @@
         <v>408452279.29417968</v>
       </c>
     </row>
-    <row r="51" spans="1:17">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>138</v>
+        <v>183</v>
       </c>
       <c r="B51" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="D51" t="s">
-        <v>140</v>
+        <v>123</v>
       </c>
       <c r="E51" t="s">
-        <v>141</v>
+        <v>124</v>
       </c>
       <c r="J51" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="K51">
         <v>240504.60431777878</v>
@@ -2963,11 +2963,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q120"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
     <col min="2" max="2" width="15.85546875" customWidth="1"/>
@@ -2981,68 +2979,68 @@
     <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" t="s">
         <v>160</v>
       </c>
-      <c r="C1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F1" t="s">
-        <v>177</v>
-      </c>
       <c r="G1" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
       <c r="H1" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="I1" t="s">
-        <v>142</v>
+        <v>125</v>
       </c>
       <c r="J1" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="K1" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="L1" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="M1" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="N1" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="O1" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="P1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
       <c r="C2" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -3072,21 +3070,21 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:17">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D3" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E3" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -3117,21 +3115,21 @@
       </c>
       <c r="Q3" s="1"/>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D4" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E4" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H4">
         <v>0.6</v>
@@ -3158,21 +3156,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D5" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E5" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="F5">
         <v>0.95</v>
@@ -3205,21 +3203,21 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D6" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E6" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -3252,21 +3250,21 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D7" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E7" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F7">
         <v>1</v>
@@ -3296,18 +3294,18 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H8">
         <v>0.8</v>
@@ -3334,21 +3332,21 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D9" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E9" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F9">
         <v>1</v>
@@ -3378,21 +3376,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C10" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D10" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E10" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F10">
         <v>1</v>
@@ -3422,21 +3420,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>149</v>
+        <v>132</v>
       </c>
       <c r="D11" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E11" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F11">
         <v>1</v>
@@ -3466,18 +3464,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E12" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -3507,18 +3505,18 @@
         <v>0.15</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E13" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -3548,18 +3546,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E14" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F14">
         <v>1</v>
@@ -3589,18 +3587,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E15" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F15">
         <v>1</v>
@@ -3630,18 +3628,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B16" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E16" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F16">
         <v>1</v>
@@ -3671,18 +3669,18 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:16">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="B17" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E17" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F17">
         <v>1</v>
@@ -3712,18 +3710,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:16">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="B18" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C18" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E18" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H18">
         <v>0.12</v>
@@ -3750,18 +3748,18 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="19" spans="1:16">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B19" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E19" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H19">
         <v>0.3</v>
@@ -3788,18 +3786,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B20" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C20" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E20" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H20">
         <v>0.4</v>
@@ -3826,18 +3824,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="21" spans="1:16">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E21" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H21">
         <v>0.5</v>
@@ -3864,18 +3862,18 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="22" spans="1:16">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C22" t="s">
-        <v>147</v>
+        <v>130</v>
       </c>
       <c r="E22" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H22">
         <v>0.6</v>
@@ -3902,18 +3900,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H23">
         <v>0.8</v>
@@ -3940,21 +3938,21 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:16">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C24" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D24" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E24" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H24">
         <v>0.7</v>
@@ -3981,18 +3979,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B25" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C25" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F25">
         <v>1</v>
@@ -4022,18 +4020,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B26" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E26" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F26">
         <v>1</v>
@@ -4063,21 +4061,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B27" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C27" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D27" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E27" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F27">
         <v>0.95</v>
@@ -4107,21 +4105,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" spans="1:16">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B28" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C28" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D28" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E28" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H28">
         <v>0.8</v>
@@ -4142,21 +4140,21 @@
         <v>0.49600000000000005</v>
       </c>
     </row>
-    <row r="29" spans="1:16">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C29" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D29" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E29" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H29">
         <v>0.9</v>
@@ -4183,18 +4181,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C30" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E30" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F30">
         <v>0.99</v>
@@ -4224,21 +4222,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:16">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D31" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E31" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H31">
         <v>0.81</v>
@@ -4265,18 +4263,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B32" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F32">
         <v>0.85</v>
@@ -4306,18 +4304,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:16">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C33" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E33" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H33">
         <v>1</v>
@@ -4344,21 +4342,21 @@
         <v>0.39</v>
       </c>
     </row>
-    <row r="34" spans="1:16">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="C34" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D34" t="s">
-        <v>156</v>
+        <v>139</v>
       </c>
       <c r="E34" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F34">
         <v>1</v>
@@ -4385,18 +4383,18 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="35" spans="1:16">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B35" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C35" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E35" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F35">
         <v>1</v>
@@ -4420,18 +4418,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:16">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E36" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F36">
         <v>1</v>
@@ -4461,21 +4459,21 @@
         <v>6.1699999999999998E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:16">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D37" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E37" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H37">
         <v>0.159</v>
@@ -4502,21 +4500,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D38" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E38" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H38">
         <v>0.75</v>
@@ -4543,18 +4541,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:16">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E39" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G39">
         <v>1</v>
@@ -4581,21 +4579,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C40" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E40" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F40">
         <v>0.71</v>
@@ -4619,21 +4617,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C41" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D41" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E41" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F41">
         <v>0.75</v>
@@ -4663,21 +4661,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:16">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D42" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E42" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F42">
         <v>1</v>
@@ -4707,18 +4705,18 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="43" spans="1:16">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F43">
         <v>1</v>
@@ -4748,18 +4746,18 @@
         <v>0.42</v>
       </c>
     </row>
-    <row r="44" spans="1:16">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>121</v>
+      </c>
+      <c r="B44" t="s">
         <v>2</v>
       </c>
-      <c r="B44" t="s">
-        <v>3</v>
-      </c>
       <c r="C44" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F44">
         <v>0.86</v>
@@ -4789,18 +4787,18 @@
         <v>0.74</v>
       </c>
     </row>
-    <row r="45" spans="1:16">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="B45" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F45">
         <v>0.86</v>
@@ -4830,21 +4828,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:16">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B46" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D46" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E46" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F46">
         <v>1</v>
@@ -4874,21 +4872,21 @@
         <v>0.86</v>
       </c>
     </row>
-    <row r="47" spans="1:16">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B47" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D47" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E47" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F47">
         <v>1</v>
@@ -4918,18 +4916,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:16">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B48" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C48" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E48" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F48">
         <v>0.65</v>
@@ -4959,21 +4957,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B49" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C49" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D49" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E49" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F49">
         <v>0.65</v>
@@ -5003,21 +5001,21 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="50" spans="1:16">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B50" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D50" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E50" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F50">
         <v>0.65</v>
@@ -5050,18 +5048,18 @@
         <v>0.35799999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:16">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="B51" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C51" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E51" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F51">
         <v>1</v>
@@ -5091,21 +5089,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:16">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B52" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C52" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D52" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E52" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -5132,21 +5130,21 @@
         <v>0.32600000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:16">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B53" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C53" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D53" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E53" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F53">
         <v>1</v>
@@ -5176,18 +5174,18 @@
         <v>5.4000000000000006E-2</v>
       </c>
     </row>
-    <row r="54" spans="1:16">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="B54" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E54" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F54">
         <v>0.7</v>
@@ -5217,18 +5215,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B55" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C55" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E55" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F55">
         <v>1</v>
@@ -5258,18 +5256,18 @@
         <v>0.30809999999999998</v>
       </c>
     </row>
-    <row r="56" spans="1:16">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="B56" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C56" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E56" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F56">
         <v>1</v>
@@ -5299,18 +5297,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B57" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C57" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E57" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F57">
         <v>0.97</v>
@@ -5340,18 +5338,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B58" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C58" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E58" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F58">
         <v>1</v>
@@ -5381,21 +5379,21 @@
         <v>0.41000000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:16">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C59" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D59" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E59" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F59">
         <v>1</v>
@@ -5425,21 +5423,21 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="60" spans="1:16">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="B60" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C60" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D60" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E60" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F60">
         <v>0.75</v>
@@ -5469,21 +5467,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:16">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B61" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C61" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D61" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E61" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F61">
         <v>1</v>
@@ -5513,18 +5511,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:16">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B62" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C62" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E62" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F62">
         <v>1</v>
@@ -5554,18 +5552,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B63" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C63" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E63" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F63">
         <v>1</v>
@@ -5595,18 +5593,18 @@
         <v>0.6</v>
       </c>
     </row>
-    <row r="64" spans="1:16">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B64" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C64" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E64" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F64">
         <v>0.95</v>
@@ -5636,21 +5634,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:16">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B65" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C65" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D65" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E65" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F65">
         <v>0.95</v>
@@ -5680,21 +5678,21 @@
         <v>0.47789999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:16">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C66" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D66" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="E66" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F66">
         <v>0.93</v>
@@ -5724,18 +5722,18 @@
         <v>0.56000000000000005</v>
       </c>
     </row>
-    <row r="67" spans="1:16">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C67" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E67" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F67">
         <v>1</v>
@@ -5765,21 +5763,21 @@
         <v>0.79</v>
       </c>
     </row>
-    <row r="68" spans="1:16">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B68" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C68" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D68" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E68" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F68">
         <v>1</v>
@@ -5809,18 +5807,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:16">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B69" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C69" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E69" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F69">
         <v>1</v>
@@ -5847,18 +5845,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B70" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E70" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F70">
         <v>1</v>
@@ -5888,21 +5886,21 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:16">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B71" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C71" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D71" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E71" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F71">
         <v>1</v>
@@ -5932,21 +5930,21 @@
         <v>6.4100000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:16">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B72" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C72" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D72" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E72" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H72">
         <v>0.7</v>
@@ -5973,18 +5971,18 @@
         <v>9.8000000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:16">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B73" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C73" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E73" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F73">
         <v>1</v>
@@ -6014,21 +6012,21 @@
         <v>0.11220000000000001</v>
       </c>
     </row>
-    <row r="74" spans="1:16">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B74" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C74" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D74" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E74" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F74">
         <v>1</v>
@@ -6058,18 +6056,18 @@
         <v>0.22870000000000001</v>
       </c>
     </row>
-    <row r="75" spans="1:16">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B75" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C75" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E75" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F75">
         <v>1</v>
@@ -6099,21 +6097,21 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="76" spans="1:16">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="B76" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D76" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E76" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F76">
         <v>1</v>
@@ -6143,21 +6141,21 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="77" spans="1:16">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="B77" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="C77" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D77" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E77" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F77">
         <v>1</v>
@@ -6187,21 +6185,21 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="78" spans="1:16">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>70</v>
+        <v>53</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
+        <v>54</v>
       </c>
       <c r="C78" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D78" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E78" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F78">
         <v>1</v>
@@ -6231,18 +6229,18 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="79" spans="1:16">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
+        <v>121</v>
+      </c>
+      <c r="B79" t="s">
         <v>2</v>
       </c>
-      <c r="B79" t="s">
-        <v>3</v>
-      </c>
       <c r="C79" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E79" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H79">
         <v>0.95</v>
@@ -6269,21 +6267,21 @@
         <v>0.84400000000000008</v>
       </c>
     </row>
-    <row r="80" spans="1:16">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C80" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E80" t="s">
-        <v>151</v>
+        <v>134</v>
       </c>
       <c r="F80">
         <v>1</v>
@@ -6316,21 +6314,21 @@
         <v>0.85299999999999998</v>
       </c>
     </row>
-    <row r="81" spans="1:16">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B81" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C81" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D81" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E81" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F81">
         <v>1</v>
@@ -6360,21 +6358,21 @@
         <v>0.55670000000000008</v>
       </c>
     </row>
-    <row r="82" spans="1:16">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B82" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D82" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E82" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H82">
         <v>1</v>
@@ -6401,21 +6399,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:16">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>17</v>
+        <v>171</v>
       </c>
       <c r="B83" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C83" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D83" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E83" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H83">
         <v>0.6</v>
@@ -6442,21 +6440,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:16">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B84" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C84" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D84" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E84" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H84">
         <v>0.95</v>
@@ -6483,18 +6481,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:16">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B85" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C85" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E85" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F85">
         <v>1</v>
@@ -6524,18 +6522,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:16">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="B86" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C86" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E86" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H86">
         <v>0.89270000000000005</v>
@@ -6562,21 +6560,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:16">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B87" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C87" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D87" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E87" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F87">
         <v>0.93100000000000005</v>
@@ -6606,18 +6604,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:16">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B88" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C88" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E88" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G88">
         <v>0.04</v>
@@ -6644,21 +6642,21 @@
         <v>0.36700000000000005</v>
       </c>
     </row>
-    <row r="89" spans="1:16">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B89" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C89" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D89" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E89" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G89">
         <v>0.7</v>
@@ -6685,18 +6683,18 @@
         <v>0.93</v>
       </c>
     </row>
-    <row r="90" spans="1:16">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B90" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C90" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E90" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F90">
         <v>1</v>
@@ -6723,18 +6721,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B91" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C91" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E91" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G91">
         <v>1</v>
@@ -6761,18 +6759,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:16">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B92" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C92" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F92">
         <v>1</v>
@@ -6799,18 +6797,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:16">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B93" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C93" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E93" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G93">
         <v>1</v>
@@ -6837,18 +6835,18 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="94" spans="1:16">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="B94" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C94" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E94" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F94">
         <v>1</v>
@@ -6878,18 +6876,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>121</v>
+      </c>
+      <c r="B95" t="s">
         <v>2</v>
       </c>
-      <c r="B95" t="s">
-        <v>3</v>
-      </c>
       <c r="C95" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E95" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F95">
         <v>1</v>
@@ -6919,21 +6917,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>7</v>
+        <v>168</v>
       </c>
       <c r="B96" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C96" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D96" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E96" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F96">
         <v>1</v>
@@ -6963,21 +6961,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>10</v>
+        <v>169</v>
       </c>
       <c r="B97" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C97" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D97" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E97" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F97">
         <v>1</v>
@@ -7007,18 +7005,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B98" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E98" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F98">
         <v>1</v>
@@ -7045,18 +7043,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>15</v>
+        <v>170</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E99" t="s">
-        <v>150</v>
+        <v>133</v>
       </c>
       <c r="G99">
         <v>1</v>
@@ -7083,21 +7081,21 @@
         <v>0.82000000000000006</v>
       </c>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>20</v>
+        <v>172</v>
       </c>
       <c r="B100" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C100" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D100" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E100" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F100">
         <v>0.87</v>
@@ -7127,18 +7125,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>24</v>
+        <v>173</v>
       </c>
       <c r="B101" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C101" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="E101" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H101">
         <v>1</v>
@@ -7165,18 +7163,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>26</v>
+        <v>174</v>
       </c>
       <c r="B102" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C102" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E102" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F102">
         <v>0.27</v>
@@ -7206,21 +7204,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>29</v>
+        <v>175</v>
       </c>
       <c r="B103" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C103" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D103" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E103" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F103">
         <v>1</v>
@@ -7250,21 +7248,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>34</v>
+        <v>176</v>
       </c>
       <c r="B104" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="C104" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D104" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E104" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -7294,21 +7292,21 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>36</v>
+        <v>177</v>
       </c>
       <c r="B105" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C105" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D105" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E105" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H105">
         <v>0.44</v>
@@ -7335,21 +7333,21 @@
         <v>0.70000000000000007</v>
       </c>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>38</v>
+        <v>178</v>
       </c>
       <c r="B106" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="C106" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D106" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E106" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -7379,18 +7377,18 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>41</v>
+        <v>179</v>
       </c>
       <c r="B107" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="C107" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E107" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F107">
         <v>0.94</v>
@@ -7420,18 +7418,18 @@
         <v>0.69000000000000006</v>
       </c>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>43</v>
+        <v>180</v>
       </c>
       <c r="B108" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C108" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E108" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F108">
         <v>0.94</v>
@@ -7461,21 +7459,21 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>45</v>
+        <v>181</v>
       </c>
       <c r="B109" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="C109" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D109" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E109" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F109">
         <v>0.94</v>
@@ -7505,21 +7503,21 @@
         <v>0.57020000000000004</v>
       </c>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>48</v>
+        <v>182</v>
       </c>
       <c r="B110" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="C110" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D110" t="s">
-        <v>154</v>
+        <v>137</v>
       </c>
       <c r="E110" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H110">
         <v>1</v>
@@ -7546,21 +7544,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>50</v>
+        <v>184</v>
       </c>
       <c r="B111" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="C111" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D111" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E111" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="F111">
         <v>0.99</v>
@@ -7587,18 +7585,18 @@
         <v>0.88300000000000001</v>
       </c>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B112" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C112" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E112" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F112">
         <v>1</v>
@@ -7628,21 +7626,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>102</v>
+        <v>85</v>
       </c>
       <c r="B113" t="s">
-        <v>103</v>
+        <v>86</v>
       </c>
       <c r="C113" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D113" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E113" t="s">
-        <v>161</v>
+        <v>144</v>
       </c>
       <c r="H113">
         <v>1</v>
@@ -7669,18 +7667,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="B114" t="s">
-        <v>106</v>
+        <v>89</v>
       </c>
       <c r="C114" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E114" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F114">
         <v>0.99</v>
@@ -7710,18 +7708,18 @@
         <v>1.52E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>107</v>
+        <v>90</v>
       </c>
       <c r="B115" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="C115" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E115" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F115">
         <v>1</v>
@@ -7751,18 +7749,18 @@
         <v>1.24E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>98</v>
+        <v>81</v>
       </c>
       <c r="B116" t="s">
-        <v>99</v>
+        <v>82</v>
       </c>
       <c r="C116" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E116" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F116">
         <v>0.66839999999999999</v>
@@ -7792,21 +7790,21 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B117" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C117" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D117" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E117" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F117">
         <v>0.2024</v>
@@ -7836,21 +7834,21 @@
         <v>0.154</v>
       </c>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B118" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C118" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D118" t="s">
-        <v>152</v>
+        <v>135</v>
       </c>
       <c r="E118" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F118">
         <v>0.66900000000000004</v>
@@ -7880,18 +7878,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B119" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C119" t="s">
-        <v>155</v>
+        <v>138</v>
       </c>
       <c r="E119" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -7921,21 +7919,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="B120" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="C120" t="s">
-        <v>153</v>
+        <v>136</v>
       </c>
       <c r="D120" t="s">
-        <v>159</v>
+        <v>142</v>
       </c>
       <c r="E120" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="F120">
         <v>0.6</v>

</xml_diff>